<commit_message>
Almost everything added.  Just going very slow and some not doubling
</commit_message>
<xml_diff>
--- a/mycsv.xlsx
+++ b/mycsv.xlsx
@@ -5625,7 +5625,7 @@
       <name val="ADP"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5653,12 +5653,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -5933,13 +5927,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5965,7 +5959,6 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -60131,9 +60124,7 @@
   </sheetPr>
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>

</xml_diff>